<commit_message>
adding localization strings for flux indicator values
</commit_message>
<xml_diff>
--- a/flux_indicators.xlsx
+++ b/flux_indicators.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11700" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11700" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="pool" sheetId="8" r:id="rId1"/>
-    <sheet name="pool_translation" sheetId="11" r:id="rId2"/>
+    <sheet name="pool_tr" sheetId="11" r:id="rId2"/>
     <sheet name="simulation_process" sheetId="7" r:id="rId3"/>
     <sheet name="flux_indicator" sheetId="1" r:id="rId4"/>
     <sheet name="flux_indicator_source" sheetId="3" r:id="rId5"/>
     <sheet name="flux_indicator_sink" sheetId="4" r:id="rId6"/>
     <sheet name="composite_flux_indicator" sheetId="5" r:id="rId7"/>
-    <sheet name="composite_flux_indicator_value" sheetId="6" r:id="rId8"/>
+    <sheet name="flux_indicator_category_tr" sheetId="13" r:id="rId8"/>
+    <sheet name="composite_flux_indicator_value" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="310">
   <si>
     <t>DeltaBiomass_AG</t>
   </si>
@@ -477,12 +478,6 @@
     <t>language</t>
   </si>
   <si>
-    <t>property</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>Softwood Merchantable</t>
   </si>
   <si>
@@ -709,6 +704,264 @@
   </si>
   <si>
     <t>Продукты</t>
+  </si>
+  <si>
+    <t>Biomass Totals</t>
+  </si>
+  <si>
+    <t>DOM Totals</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Ecosystem Indicators</t>
+  </si>
+  <si>
+    <t>Ecosystem to Forest Products</t>
+  </si>
+  <si>
+    <t>Release to Atmostphere</t>
+  </si>
+  <si>
+    <t>Emissions By Source</t>
+  </si>
+  <si>
+    <t>Emissions By Gas</t>
+  </si>
+  <si>
+    <t>Biomass Emissions By Gas</t>
+  </si>
+  <si>
+    <t>DOM Emissions By Gas</t>
+  </si>
+  <si>
+    <t>Disturbance Transfers</t>
+  </si>
+  <si>
+    <t>Stock Changes</t>
+  </si>
+  <si>
+    <t>Ecosystem Transfers</t>
+  </si>
+  <si>
+    <t>Emissions</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>SubCategoryName</t>
+  </si>
+  <si>
+    <t>flux_indicator_category_id</t>
+  </si>
+  <si>
+    <t>pl-PL</t>
+  </si>
+  <si>
+    <t>Delta écosystème total</t>
+  </si>
+  <si>
+    <t>Дельта всей экосистемы</t>
+  </si>
+  <si>
+    <t>Całkowita zmiana ekosystemu</t>
+  </si>
+  <si>
+    <t>Cambio total en ecosistema</t>
+  </si>
+  <si>
+    <t>Delta biomasse totale</t>
+  </si>
+  <si>
+    <t>Cambio total en biomasa</t>
+  </si>
+  <si>
+    <t>Zmiana całkowitej biomasy</t>
+  </si>
+  <si>
+    <t>Дельта общей биомассы</t>
+  </si>
+  <si>
+    <t>Cambio total en MOM</t>
+  </si>
+  <si>
+    <t>Delta MOM totale</t>
+  </si>
+  <si>
+    <t>Zmiana całkowitej, rozpuszczonej martwej materii organicznej (DOM)</t>
+  </si>
+  <si>
+    <t>Дельта общего МОВ</t>
+  </si>
+  <si>
+    <t>Productivité du biome nette (PBN)</t>
+  </si>
+  <si>
+    <t>Produkcja biomu netto (NBP)</t>
+  </si>
+  <si>
+    <t>Productividad de bioma neta (PBN)</t>
+  </si>
+  <si>
+    <t>Чистая продуктивность биома (ЧПБ)</t>
+  </si>
+  <si>
+    <t>Produkcyjność ekosystemu netto (NEP)</t>
+  </si>
+  <si>
+    <t>Productivité écosystémique nette (PEN)</t>
+  </si>
+  <si>
+    <t>Чистая продуктивность экосистемы (ЧПЭ)</t>
+  </si>
+  <si>
+    <t>Productividad neta del ecosistema (PNE)</t>
+  </si>
+  <si>
+    <t>Produkcja podstawowa netto (NPP)</t>
+  </si>
+  <si>
+    <t>Чистая первичная продуктивность (ЧПП)</t>
+  </si>
+  <si>
+    <t>Productivité primaire nette (PPN)</t>
+  </si>
+  <si>
+    <t>Productividad primaria neta (PPN)</t>
+  </si>
+  <si>
+    <t>Croissance nette</t>
+  </si>
+  <si>
+    <t>Чистый рост</t>
+  </si>
+  <si>
+    <t>Crecimiento neto</t>
+  </si>
+  <si>
+    <t>Wzrost netto</t>
+  </si>
+  <si>
+    <t>Opad listowia netto</t>
+  </si>
+  <si>
+    <t>Hojarasca neta</t>
+  </si>
+  <si>
+    <t>Chute de litière nette</t>
+  </si>
+  <si>
+    <t>Чистый опад</t>
+  </si>
+  <si>
+    <t>Chute de litière totale</t>
+  </si>
+  <si>
+    <t>Всего опада</t>
+  </si>
+  <si>
+    <t>Hojarasca total</t>
+  </si>
+  <si>
+    <t>Całkowity opad listowia</t>
+  </si>
+  <si>
+    <t>Emisje rozkładu</t>
+  </si>
+  <si>
+    <t>Emisiones de descomposición</t>
+  </si>
+  <si>
+    <t>Выбросы от разложения</t>
+  </si>
+  <si>
+    <t>Rejets de décomposition</t>
+  </si>
+  <si>
+    <t>Całkowite pozyskanie (biomasa + posusz)</t>
+  </si>
+  <si>
+    <t>Explotación total (biomasa + árboles muertos)</t>
+  </si>
+  <si>
+    <t>Общий урожай (биомасса + валеж)</t>
+  </si>
+  <si>
+    <t>Récolte totale (biomasse + chicots)</t>
+  </si>
+  <si>
+    <t>Récolte totale (biomasse)</t>
+  </si>
+  <si>
+    <t>Общий урожай (биомасса)</t>
+  </si>
+  <si>
+    <t>Explotación total (biomasa)</t>
+  </si>
+  <si>
+    <t>Całkowite pozyskanie (biomasa)</t>
+  </si>
+  <si>
+    <t>Récolte totale (chicots)</t>
+  </si>
+  <si>
+    <t>Общий урожай (валеж)</t>
+  </si>
+  <si>
+    <t>Explotación total (árboles muertos)</t>
+  </si>
+  <si>
+    <t>Całkowite pozyskanie (posusz)</t>
+  </si>
+  <si>
+    <t>Récolte de résineux (biomasse)</t>
+  </si>
+  <si>
+    <t>Урожай хвойных (биомасса)</t>
+  </si>
+  <si>
+    <t>Explotación de coníferas (biomasa)</t>
+  </si>
+  <si>
+    <t>Pozyskanie iglastych (biomasa)</t>
+  </si>
+  <si>
+    <t>Récolte de feuillus (biomasse)</t>
+  </si>
+  <si>
+    <t>Урожай лиственных (биомасса)</t>
+  </si>
+  <si>
+    <t>Explotación de caducifolios (biomasa)</t>
+  </si>
+  <si>
+    <t>Pozyskanie liściastych (biomasa)</t>
+  </si>
+  <si>
+    <t>Récolte de résineux (chicots)</t>
+  </si>
+  <si>
+    <t>Урожай хвойных (валеж)</t>
+  </si>
+  <si>
+    <t>Explotación de coníferas (árboles muertos)</t>
+  </si>
+  <si>
+    <t>Pozyskanie iglastych (posusz)</t>
+  </si>
+  <si>
+    <t>Récolte de feuillus (chicots)</t>
+  </si>
+  <si>
+    <t>Урожай лиственных (валеж)</t>
+  </si>
+  <si>
+    <t>Explotación de caducifolios (árboles muertos)</t>
+  </si>
+  <si>
+    <t>Pozyskanie liściastych (posusz)</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1458,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A28"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,35 +1697,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G96" sqref="G95:G96"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C1" t="s">
         <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1483,13 +1734,10 @@
         <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1499,14 +1747,11 @@
       <c r="C3" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1516,14 +1761,11 @@
       <c r="C4" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1533,14 +1775,11 @@
       <c r="C5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1550,14 +1789,11 @@
       <c r="C6" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1567,14 +1803,11 @@
       <c r="C7" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1584,14 +1817,11 @@
       <c r="C8" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1601,14 +1831,11 @@
       <c r="C9" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1618,14 +1845,11 @@
       <c r="C10" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1635,14 +1859,11 @@
       <c r="C11" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1652,14 +1873,11 @@
       <c r="C12" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1669,14 +1887,11 @@
       <c r="C13" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1686,14 +1901,11 @@
       <c r="C14" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1703,14 +1915,11 @@
       <c r="C15" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1720,14 +1929,11 @@
       <c r="C16" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1737,14 +1943,11 @@
       <c r="C17" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1754,14 +1957,11 @@
       <c r="C18" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1771,14 +1971,11 @@
       <c r="C19" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1788,14 +1985,11 @@
       <c r="C20" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1805,14 +1999,11 @@
       <c r="C21" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1822,14 +2013,11 @@
       <c r="C22" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1839,14 +2027,11 @@
       <c r="C23" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1856,14 +2041,11 @@
       <c r="C24" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1873,14 +2055,11 @@
       <c r="C25" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1890,14 +2069,11 @@
       <c r="C26" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D26" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1907,14 +2083,11 @@
       <c r="C27" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1925,13 +2098,10 @@
         <v>144</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1941,14 +2111,11 @@
       <c r="C29" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1958,14 +2125,11 @@
       <c r="C30" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1975,14 +2139,11 @@
       <c r="C31" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1992,14 +2153,11 @@
       <c r="C32" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2009,14 +2167,11 @@
       <c r="C33" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2026,14 +2181,11 @@
       <c r="C34" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2043,14 +2195,11 @@
       <c r="C35" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2060,14 +2209,11 @@
       <c r="C36" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2077,14 +2223,11 @@
       <c r="C37" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2094,14 +2237,11 @@
       <c r="C38" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2111,14 +2251,11 @@
       <c r="C39" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2128,14 +2265,11 @@
       <c r="C40" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2145,14 +2279,11 @@
       <c r="C41" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E41" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2162,14 +2293,11 @@
       <c r="C42" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2179,14 +2307,11 @@
       <c r="C43" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2196,14 +2321,11 @@
       <c r="C44" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2213,14 +2335,11 @@
       <c r="C45" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2230,14 +2349,11 @@
       <c r="C46" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2247,14 +2363,11 @@
       <c r="C47" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2264,14 +2377,11 @@
       <c r="C48" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E48" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2281,14 +2391,11 @@
       <c r="C49" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="D49" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2298,14 +2405,11 @@
       <c r="C50" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="D50" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2315,14 +2419,11 @@
       <c r="C51" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="D51" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2332,14 +2433,11 @@
       <c r="C52" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D52" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2349,14 +2447,11 @@
       <c r="C53" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2366,14 +2461,11 @@
       <c r="C54" t="s">
         <v>145</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2383,14 +2475,11 @@
       <c r="C55" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E55" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2400,14 +2489,11 @@
       <c r="C56" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E56" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2417,14 +2503,11 @@
       <c r="C57" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E57" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2434,14 +2517,11 @@
       <c r="C58" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E58" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2451,14 +2531,11 @@
       <c r="C59" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E59" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2468,14 +2545,11 @@
       <c r="C60" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E60" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2485,14 +2559,11 @@
       <c r="C61" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E61" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2502,14 +2573,11 @@
       <c r="C62" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E62" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2519,14 +2587,11 @@
       <c r="C63" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E63" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2536,14 +2601,11 @@
       <c r="C64" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E64" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2553,14 +2615,11 @@
       <c r="C65" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E65" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2570,14 +2629,11 @@
       <c r="C66" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E66" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2587,14 +2643,11 @@
       <c r="C67" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E67" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2604,14 +2657,11 @@
       <c r="C68" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E68" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2621,14 +2671,11 @@
       <c r="C69" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E69" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2638,14 +2685,11 @@
       <c r="C70" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E70" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2655,14 +2699,11 @@
       <c r="C71" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E71" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2672,14 +2713,11 @@
       <c r="C72" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E72" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2689,14 +2727,11 @@
       <c r="C73" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E73" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -2706,14 +2741,11 @@
       <c r="C74" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E74" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -2723,14 +2755,11 @@
       <c r="C75" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E75" t="s">
+      <c r="D75" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -2740,14 +2769,11 @@
       <c r="C76" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="D76" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -2757,14 +2783,11 @@
       <c r="C77" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E77" t="s">
+      <c r="D77" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -2774,14 +2797,11 @@
       <c r="C78" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E78" t="s">
+      <c r="D78" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -2791,14 +2811,11 @@
       <c r="C79" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E79" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -2809,13 +2826,10 @@
         <v>146</v>
       </c>
       <c r="D80" t="s">
-        <v>33</v>
-      </c>
-      <c r="E80" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -2825,14 +2839,11 @@
       <c r="C81" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E81" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -2842,14 +2853,11 @@
       <c r="C82" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E82" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -2859,14 +2867,11 @@
       <c r="C83" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E83" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -2876,14 +2881,11 @@
       <c r="C84" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E84" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -2893,14 +2895,11 @@
       <c r="C85" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E85" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -2910,14 +2909,11 @@
       <c r="C86" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E86" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -2927,14 +2923,11 @@
       <c r="C87" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E87" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -2944,14 +2937,11 @@
       <c r="C88" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E88" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -2961,14 +2951,11 @@
       <c r="C89" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E89" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -2978,14 +2965,11 @@
       <c r="C90" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E90" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -2995,14 +2979,11 @@
       <c r="C91" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E91" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -3012,14 +2993,11 @@
       <c r="C92" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E92" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -3029,14 +3007,11 @@
       <c r="C93" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E93" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -3046,14 +3021,11 @@
       <c r="C94" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E94" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -3063,14 +3035,11 @@
       <c r="C95" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E95" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -3080,14 +3049,11 @@
       <c r="C96" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E96" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -3097,14 +3063,11 @@
       <c r="C97" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E97" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -3114,14 +3077,11 @@
       <c r="C98" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D98" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E98" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -3131,14 +3091,11 @@
       <c r="C99" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E99" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -3148,14 +3105,11 @@
       <c r="C100" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E100" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -3165,14 +3119,11 @@
       <c r="C101" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E101" t="s">
+      <c r="D101" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -3182,14 +3133,11 @@
       <c r="C102" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E102" t="s">
+      <c r="D102" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -3199,14 +3147,11 @@
       <c r="C103" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E103" t="s">
+      <c r="D103" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -3216,14 +3161,11 @@
       <c r="C104" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="D104" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -3233,11 +3175,8 @@
       <c r="C105" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E105" t="s">
-        <v>225</v>
+      <c r="D105" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -3299,7 +3238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -4114,7 +4053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X214"/>
   <sheetViews>
-    <sheetView topLeftCell="A185" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
@@ -7403,7 +7342,7 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A71" sqref="A71:D71"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8485,155 +8424,363 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" t="s">
+        <v>258</v>
+      </c>
+      <c r="F6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" t="s">
+        <v>268</v>
+      </c>
+      <c r="E7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8" t="s">
+        <v>270</v>
+      </c>
+      <c r="F8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>274</v>
+      </c>
+      <c r="D9" t="s">
+        <v>276</v>
+      </c>
+      <c r="E9" t="s">
+        <v>277</v>
+      </c>
+      <c r="F9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D10" t="s">
+        <v>279</v>
+      </c>
+      <c r="E10" t="s">
+        <v>278</v>
+      </c>
+      <c r="F10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" t="s">
+        <v>283</v>
+      </c>
+      <c r="E11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D12" t="s">
+        <v>288</v>
+      </c>
+      <c r="E12" t="s">
+        <v>289</v>
+      </c>
+      <c r="F12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D13" t="s">
+        <v>292</v>
+      </c>
+      <c r="E13" t="s">
+        <v>293</v>
+      </c>
+      <c r="F13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E14" t="s">
+        <v>297</v>
+      </c>
+      <c r="F14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>298</v>
+      </c>
+      <c r="D15" t="s">
+        <v>300</v>
+      </c>
+      <c r="E15" t="s">
+        <v>301</v>
+      </c>
+      <c r="F15" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>302</v>
+      </c>
+      <c r="D16" t="s">
+        <v>304</v>
+      </c>
+      <c r="E16" t="s">
+        <v>305</v>
+      </c>
+      <c r="F16" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>306</v>
+      </c>
+      <c r="D17" t="s">
+        <v>308</v>
+      </c>
+      <c r="E17" t="s">
+        <v>309</v>
+      </c>
+      <c r="F17" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -8641,7 +8788,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -8649,7 +8796,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -8657,7 +8804,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -8665,7 +8812,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -8673,7 +8820,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -8681,7 +8828,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -8689,7 +8836,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -8697,7 +8844,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -8705,7 +8852,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -8713,7 +8860,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -8721,7 +8868,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -8729,7 +8876,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -8737,7 +8884,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -8745,7 +8892,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>33</v>
       </c>
@@ -8753,7 +8900,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>34</v>
       </c>
@@ -8761,7 +8908,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>35</v>
       </c>
@@ -8769,7 +8916,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>36</v>
       </c>
@@ -8777,7 +8924,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>37</v>
       </c>
@@ -8785,7 +8932,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>38</v>
       </c>
@@ -8793,7 +8940,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>39</v>
       </c>
@@ -8801,7 +8948,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>40</v>
       </c>
@@ -8809,7 +8956,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>41</v>
       </c>
@@ -8817,7 +8964,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>42</v>
       </c>
@@ -8825,7 +8972,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43</v>
       </c>
@@ -8833,7 +8980,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44</v>
       </c>
@@ -8841,7 +8988,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45</v>
       </c>
@@ -8849,7 +8996,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>46</v>
       </c>
@@ -8857,12 +9004,24 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>47</v>
       </c>
       <c r="B46" t="s">
         <v>76</v>
+      </c>
+      <c r="C46" t="s">
+        <v>254</v>
+      </c>
+      <c r="D46" t="s">
+        <v>256</v>
+      </c>
+      <c r="E46" t="s">
+        <v>255</v>
+      </c>
+      <c r="F46" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -8872,10 +9031,148 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I203"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>